<commit_message>
update up to 22
</commit_message>
<xml_diff>
--- a/pali-class/vocab/vocab-class10.xlsx
+++ b/pali-class/vocab/vocab-class10.xlsx
@@ -46,24 +46,24 @@
     <t>amu</t>
   </si>
   <si>
+    <t>anāpucchanta</t>
+  </si>
+  <si>
+    <t>passanta</t>
+  </si>
+  <si>
+    <t>jānanta</t>
+  </si>
+  <si>
+    <t>samanupassanta</t>
+  </si>
+  <si>
+    <t>tiṭṭhanta 1</t>
+  </si>
+  <si>
     <t>anussaranta</t>
   </si>
   <si>
-    <t>anāpucchanta</t>
-  </si>
-  <si>
-    <t>passanta</t>
-  </si>
-  <si>
-    <t>jānanta</t>
-  </si>
-  <si>
-    <t>samanupassanta</t>
-  </si>
-  <si>
-    <t>tiṭṭhanta 1</t>
-  </si>
-  <si>
     <t>gacchanta</t>
   </si>
   <si>
@@ -94,27 +94,297 @@
     <t>ākaṅkhamāna</t>
   </si>
   <si>
+    <t>vinaya 1</t>
+  </si>
+  <si>
+    <t>dhamma 03</t>
+  </si>
+  <si>
+    <t>pariyāya 4</t>
+  </si>
+  <si>
+    <t>manussa</t>
+  </si>
+  <si>
+    <t>deva 1</t>
+  </si>
+  <si>
+    <t>papañca</t>
+  </si>
+  <si>
+    <t>saṅghādisesa 2</t>
+  </si>
+  <si>
+    <t>vasa 2</t>
+  </si>
+  <si>
+    <t>vaccha 1</t>
+  </si>
+  <si>
+    <t>puggala</t>
+  </si>
+  <si>
+    <t>āsaya 2</t>
+  </si>
+  <si>
+    <t>dhamma 01</t>
+  </si>
+  <si>
+    <t>uposatha 1</t>
+  </si>
+  <si>
+    <t>bhava 2</t>
+  </si>
+  <si>
+    <t>vassa 2</t>
+  </si>
+  <si>
+    <t>āvāsa 1</t>
+  </si>
+  <si>
+    <t>antarāya</t>
+  </si>
+  <si>
+    <t>moggallāna 1</t>
+  </si>
+  <si>
     <t>dhamma 15</t>
   </si>
   <si>
+    <t>saṃvara 2</t>
+  </si>
+  <si>
+    <t>magga 1</t>
+  </si>
+  <si>
+    <t>putta 1</t>
+  </si>
+  <si>
+    <t>māsa 2</t>
+  </si>
+  <si>
+    <t>bhoga 1</t>
+  </si>
+  <si>
+    <t>paccaya 2</t>
+  </si>
+  <si>
+    <t>purisa 1</t>
+  </si>
+  <si>
+    <t>samaya 1</t>
+  </si>
+  <si>
+    <t>attha 01</t>
+  </si>
+  <si>
+    <t>sāriputta</t>
+  </si>
+  <si>
+    <t>pañha 2</t>
+  </si>
+  <si>
+    <t>ābādha</t>
+  </si>
+  <si>
+    <t>saṅkhāra 3</t>
+  </si>
+  <si>
     <t>khattiya 2</t>
   </si>
   <si>
+    <t>phassa 1</t>
+  </si>
+  <si>
+    <t>puthujjana</t>
+  </si>
+  <si>
+    <t>daṇḍa 1</t>
+  </si>
+  <si>
     <t>magga 2</t>
   </si>
   <si>
     <t>dhamma 06</t>
   </si>
   <si>
+    <t>rasa 1</t>
+  </si>
+  <si>
+    <t>māṇava</t>
+  </si>
+  <si>
     <t>loka 1</t>
   </si>
   <si>
     <t>kāma 3</t>
   </si>
   <si>
+    <t>yāma 1</t>
+  </si>
+  <si>
+    <t>pāda 1</t>
+  </si>
+  <si>
+    <t>bheda 2</t>
+  </si>
+  <si>
+    <t>parikkhāra 1</t>
+  </si>
+  <si>
+    <t>patha 2</t>
+  </si>
+  <si>
+    <t>ānanda 2</t>
+  </si>
+  <si>
+    <t>attha 02</t>
+  </si>
+  <si>
+    <t>ānisaṃsa 1</t>
+  </si>
+  <si>
+    <t>vāta 1</t>
+  </si>
+  <si>
+    <t>sakuṇa</t>
+  </si>
+  <si>
+    <t>paṇḍita 2</t>
+  </si>
+  <si>
+    <t>hattha 1</t>
+  </si>
+  <si>
+    <t>satta 2</t>
+  </si>
+  <si>
+    <t>niraya</t>
+  </si>
+  <si>
+    <t>vinipāta</t>
+  </si>
+  <si>
+    <t>māna 1</t>
+  </si>
+  <si>
+    <t>kāya 2</t>
+  </si>
+  <si>
+    <t>saṅgha 1</t>
+  </si>
+  <si>
+    <t>udapāna</t>
+  </si>
+  <si>
+    <t>upāyāsa</t>
+  </si>
+  <si>
+    <t>parideva</t>
+  </si>
+  <si>
+    <t>soka</t>
+  </si>
+  <si>
+    <t>dosa 1</t>
+  </si>
+  <si>
+    <t>rāga 1</t>
+  </si>
+  <si>
+    <t>bheda 3</t>
+  </si>
+  <si>
     <t>sāvaka</t>
   </si>
   <si>
+    <t>paccaya 1</t>
+  </si>
+  <si>
+    <t>uccāra</t>
+  </si>
+  <si>
+    <t>passāva</t>
+  </si>
+  <si>
+    <t>khaya</t>
+  </si>
+  <si>
+    <t>āsava 2</t>
+  </si>
+  <si>
+    <t>nīvaraṇa 1</t>
+  </si>
+  <si>
+    <t>sekha</t>
+  </si>
+  <si>
+    <t>dhamma 02</t>
+  </si>
+  <si>
+    <t>samatha 1</t>
+  </si>
+  <si>
+    <t>pallaṅka 2</t>
+  </si>
+  <si>
+    <t>anālaya 1</t>
+  </si>
+  <si>
+    <t>paṭinissagga</t>
+  </si>
+  <si>
+    <t>cāga 1</t>
+  </si>
+  <si>
+    <t>āloka</t>
+  </si>
+  <si>
+    <t>rāhula</t>
+  </si>
+  <si>
+    <t>gandha 1</t>
+  </si>
+  <si>
+    <t>gotama</t>
+  </si>
+  <si>
+    <t>samaṇa 1</t>
+  </si>
+  <si>
+    <t>nirodha</t>
+  </si>
+  <si>
+    <t>virāga 1</t>
+  </si>
+  <si>
+    <t>samudaya 1</t>
+  </si>
+  <si>
+    <t>khandha 1</t>
+  </si>
+  <si>
+    <t>sambodha</t>
+  </si>
+  <si>
+    <t>upasama</t>
+  </si>
+  <si>
+    <t>pamāda</t>
+  </si>
+  <si>
+    <t>māra</t>
+  </si>
+  <si>
+    <t>brāhmaṇa 1</t>
+  </si>
+  <si>
+    <t>ogha 1</t>
+  </si>
+  <si>
+    <t>sakka 3</t>
+  </si>
+  <si>
     <t>adhigama 1</t>
   </si>
   <si>
@@ -124,6 +394,48 @@
     <t>samatikkama</t>
   </si>
   <si>
+    <t>saṃvara 1</t>
+  </si>
+  <si>
+    <t>amanasikāra 1</t>
+  </si>
+  <si>
+    <t>uddesa 1</t>
+  </si>
+  <si>
+    <t>chanda 2</t>
+  </si>
+  <si>
+    <t>khandha 3</t>
+  </si>
+  <si>
+    <t>brāhmaṇa 2</t>
+  </si>
+  <si>
+    <t>sota 1</t>
+  </si>
+  <si>
+    <t>vūpasama 1</t>
+  </si>
+  <si>
+    <t>loka 2</t>
+  </si>
+  <si>
+    <t>samudda</t>
+  </si>
+  <si>
+    <t>asura</t>
+  </si>
+  <si>
+    <t>saṅkhāra 1</t>
+  </si>
+  <si>
+    <t>virāga 2</t>
+  </si>
+  <si>
+    <t>āhāra 1</t>
+  </si>
+  <si>
     <t>visesa 1</t>
   </si>
   <si>
@@ -136,318 +448,6 @@
     <t>kesa</t>
   </si>
   <si>
-    <t>vinaya 1</t>
-  </si>
-  <si>
-    <t>dhamma 03</t>
-  </si>
-  <si>
-    <t>pariyāya 4</t>
-  </si>
-  <si>
-    <t>manussa</t>
-  </si>
-  <si>
-    <t>deva 1</t>
-  </si>
-  <si>
-    <t>papañca</t>
-  </si>
-  <si>
-    <t>saṅghādisesa 2</t>
-  </si>
-  <si>
-    <t>vasa 2</t>
-  </si>
-  <si>
-    <t>vaccha 1</t>
-  </si>
-  <si>
-    <t>puggala</t>
-  </si>
-  <si>
-    <t>āsaya 2</t>
-  </si>
-  <si>
-    <t>dhamma 01</t>
-  </si>
-  <si>
-    <t>uposatha 1</t>
-  </si>
-  <si>
-    <t>bhava 2</t>
-  </si>
-  <si>
-    <t>vassa 2</t>
-  </si>
-  <si>
-    <t>āvāsa 1</t>
-  </si>
-  <si>
-    <t>antarāya</t>
-  </si>
-  <si>
-    <t>moggallāna 1</t>
-  </si>
-  <si>
-    <t>saṃvara 2</t>
-  </si>
-  <si>
-    <t>māsa 2</t>
-  </si>
-  <si>
-    <t>magga 1</t>
-  </si>
-  <si>
-    <t>putta 1</t>
-  </si>
-  <si>
-    <t>bhoga 1</t>
-  </si>
-  <si>
-    <t>paccaya 2</t>
-  </si>
-  <si>
-    <t>samaya 1</t>
-  </si>
-  <si>
-    <t>purisa 1</t>
-  </si>
-  <si>
-    <t>attha 01</t>
-  </si>
-  <si>
-    <t>sāriputta</t>
-  </si>
-  <si>
-    <t>pañha 2</t>
-  </si>
-  <si>
-    <t>ābādha</t>
-  </si>
-  <si>
-    <t>saṅkhāra 3</t>
-  </si>
-  <si>
-    <t>phassa 1</t>
-  </si>
-  <si>
-    <t>puthujjana</t>
-  </si>
-  <si>
-    <t>daṇḍa 1</t>
-  </si>
-  <si>
-    <t>rasa 1</t>
-  </si>
-  <si>
-    <t>māṇava</t>
-  </si>
-  <si>
-    <t>yāma 1</t>
-  </si>
-  <si>
-    <t>pāda 1</t>
-  </si>
-  <si>
-    <t>bheda 2</t>
-  </si>
-  <si>
-    <t>parikkhāra 1</t>
-  </si>
-  <si>
-    <t>patha 2</t>
-  </si>
-  <si>
-    <t>ānanda 2</t>
-  </si>
-  <si>
-    <t>attha 02</t>
-  </si>
-  <si>
-    <t>ānisaṃsa 1</t>
-  </si>
-  <si>
-    <t>vāta 1</t>
-  </si>
-  <si>
-    <t>sakuṇa</t>
-  </si>
-  <si>
-    <t>paṇḍita 2</t>
-  </si>
-  <si>
-    <t>hattha 1</t>
-  </si>
-  <si>
-    <t>satta 2</t>
-  </si>
-  <si>
-    <t>niraya</t>
-  </si>
-  <si>
-    <t>vinipāta</t>
-  </si>
-  <si>
-    <t>māna 1</t>
-  </si>
-  <si>
-    <t>kāya 2</t>
-  </si>
-  <si>
-    <t>saṅgha 1</t>
-  </si>
-  <si>
-    <t>udapāna</t>
-  </si>
-  <si>
-    <t>upāyāsa</t>
-  </si>
-  <si>
-    <t>parideva</t>
-  </si>
-  <si>
-    <t>soka</t>
-  </si>
-  <si>
-    <t>dosa 1</t>
-  </si>
-  <si>
-    <t>rāga 1</t>
-  </si>
-  <si>
-    <t>bheda 3</t>
-  </si>
-  <si>
-    <t>paccaya 1</t>
-  </si>
-  <si>
-    <t>uccāra</t>
-  </si>
-  <si>
-    <t>passāva</t>
-  </si>
-  <si>
-    <t>khaya</t>
-  </si>
-  <si>
-    <t>āsava 2</t>
-  </si>
-  <si>
-    <t>nīvaraṇa 1</t>
-  </si>
-  <si>
-    <t>sekha</t>
-  </si>
-  <si>
-    <t>dhamma 02</t>
-  </si>
-  <si>
-    <t>samatha 1</t>
-  </si>
-  <si>
-    <t>pallaṅka 2</t>
-  </si>
-  <si>
-    <t>anālaya 1</t>
-  </si>
-  <si>
-    <t>paṭinissagga</t>
-  </si>
-  <si>
-    <t>cāga 1</t>
-  </si>
-  <si>
-    <t>āloka</t>
-  </si>
-  <si>
-    <t>rāhula</t>
-  </si>
-  <si>
-    <t>gandha 1</t>
-  </si>
-  <si>
-    <t>samudaya 1</t>
-  </si>
-  <si>
-    <t>khandha 1</t>
-  </si>
-  <si>
-    <t>gotama</t>
-  </si>
-  <si>
-    <t>samaṇa 1</t>
-  </si>
-  <si>
-    <t>nirodha</t>
-  </si>
-  <si>
-    <t>virāga 1</t>
-  </si>
-  <si>
-    <t>sambodha</t>
-  </si>
-  <si>
-    <t>upasama</t>
-  </si>
-  <si>
-    <t>pamāda</t>
-  </si>
-  <si>
-    <t>māra</t>
-  </si>
-  <si>
-    <t>brāhmaṇa 1</t>
-  </si>
-  <si>
-    <t>ogha 1</t>
-  </si>
-  <si>
-    <t>sakka 3</t>
-  </si>
-  <si>
-    <t>saṃvara 1</t>
-  </si>
-  <si>
-    <t>amanasikāra 1</t>
-  </si>
-  <si>
-    <t>uddesa 1</t>
-  </si>
-  <si>
-    <t>chanda 2</t>
-  </si>
-  <si>
-    <t>khandha 3</t>
-  </si>
-  <si>
-    <t>brāhmaṇa 2</t>
-  </si>
-  <si>
-    <t>sota 1</t>
-  </si>
-  <si>
-    <t>vūpasama 1</t>
-  </si>
-  <si>
-    <t>loka 2</t>
-  </si>
-  <si>
-    <t>samudda</t>
-  </si>
-  <si>
-    <t>asura</t>
-  </si>
-  <si>
-    <t>saṅkhāra 1</t>
-  </si>
-  <si>
-    <t>virāga 2</t>
-  </si>
-  <si>
-    <t>āhāra 1</t>
-  </si>
-  <si>
     <t>sahāya</t>
   </si>
   <si>
@@ -568,165 +568,165 @@
     <t>kosalā</t>
   </si>
   <si>
+    <t>punabbhava</t>
+  </si>
+  <si>
     <t>pātimokkha 2</t>
   </si>
   <si>
-    <t>punabbhava</t>
-  </si>
-  <si>
     <t>vibhaṅga 1</t>
   </si>
   <si>
+    <t>pajahati</t>
+  </si>
+  <si>
+    <t>paṭisevati 1</t>
+  </si>
+  <si>
+    <t>uddharati 2</t>
+  </si>
+  <si>
+    <t>bandhati 1</t>
+  </si>
+  <si>
+    <t>passa 5</t>
+  </si>
+  <si>
+    <t>tiṭṭhati 3</t>
+  </si>
+  <si>
+    <t>abhivaḍḍhati</t>
+  </si>
+  <si>
+    <t>vadati 1</t>
+  </si>
+  <si>
+    <t>pabbajati</t>
+  </si>
+  <si>
+    <t>uddisati 1</t>
+  </si>
+  <si>
     <t>pakkamati 1</t>
   </si>
   <si>
+    <t>ārabhati 1</t>
+  </si>
+  <si>
+    <t>icchati 1</t>
+  </si>
+  <si>
+    <t>rakkhati 2</t>
+  </si>
+  <si>
+    <t>upasaṅkamati</t>
+  </si>
+  <si>
+    <t>bhāsati 1</t>
+  </si>
+  <si>
+    <t>yācati 1</t>
+  </si>
+  <si>
+    <t>harati 2</t>
+  </si>
+  <si>
+    <t>paṭilabhati</t>
+  </si>
+  <si>
+    <t>passasati</t>
+  </si>
+  <si>
+    <t>assasati</t>
+  </si>
+  <si>
+    <t>ākaṅkhati</t>
+  </si>
+  <si>
+    <t>gaṇhati 1</t>
+  </si>
+  <si>
     <t>bhaṇati 1</t>
   </si>
   <si>
+    <t>ovadati</t>
+  </si>
+  <si>
+    <t>passati 2</t>
+  </si>
+  <si>
+    <t>jahati 1</t>
+  </si>
+  <si>
+    <t>sikkhati 2</t>
+  </si>
+  <si>
+    <t>paṭisevati 2</t>
+  </si>
+  <si>
+    <t>pavaḍḍhati 1</t>
+  </si>
+  <si>
+    <t>nikkhipati 3</t>
+  </si>
+  <si>
+    <t>bhajati 1</t>
+  </si>
+  <si>
+    <t>arahati 3</t>
+  </si>
+  <si>
     <t>vattati 1</t>
   </si>
   <si>
+    <t>labhati</t>
+  </si>
+  <si>
+    <t>anussarati 1</t>
+  </si>
+  <si>
+    <t>nisīdati</t>
+  </si>
+  <si>
+    <t>bhavati 1</t>
+  </si>
+  <si>
+    <t>khādati</t>
+  </si>
+  <si>
     <t>pucchati</t>
   </si>
   <si>
+    <t>saṃvattati</t>
+  </si>
+  <si>
+    <t>gacchati 1</t>
+  </si>
+  <si>
+    <t>padahati 1</t>
+  </si>
+  <si>
+    <t>vāyamati</t>
+  </si>
+  <si>
+    <t>adhigacchati</t>
+  </si>
+  <si>
+    <t>abhiramati</t>
+  </si>
+  <si>
+    <t>pavisati</t>
+  </si>
+  <si>
+    <t>viharati 1</t>
+  </si>
+  <si>
+    <t>vaḍḍhati</t>
+  </si>
+  <si>
     <t>kappati</t>
   </si>
   <si>
-    <t>pajahati</t>
-  </si>
-  <si>
-    <t>paṭisevati 1</t>
-  </si>
-  <si>
-    <t>uddharati 2</t>
-  </si>
-  <si>
-    <t>bandhati 1</t>
-  </si>
-  <si>
-    <t>passa 5</t>
-  </si>
-  <si>
-    <t>tiṭṭhati 3</t>
-  </si>
-  <si>
-    <t>pabbajati</t>
-  </si>
-  <si>
-    <t>abhivaḍḍhati</t>
-  </si>
-  <si>
-    <t>vadati 1</t>
-  </si>
-  <si>
-    <t>uddisati 1</t>
-  </si>
-  <si>
-    <t>ārabhati 1</t>
-  </si>
-  <si>
-    <t>icchati 1</t>
-  </si>
-  <si>
-    <t>rakkhati 2</t>
-  </si>
-  <si>
-    <t>upasaṅkamati</t>
-  </si>
-  <si>
-    <t>bhāsati 1</t>
-  </si>
-  <si>
-    <t>yācati 1</t>
-  </si>
-  <si>
-    <t>harati 2</t>
-  </si>
-  <si>
-    <t>paṭilabhati</t>
-  </si>
-  <si>
-    <t>passasati</t>
-  </si>
-  <si>
-    <t>assasati</t>
-  </si>
-  <si>
-    <t>ākaṅkhati</t>
-  </si>
-  <si>
-    <t>gaṇhati 1</t>
-  </si>
-  <si>
-    <t>ovadati</t>
-  </si>
-  <si>
-    <t>passati 2</t>
-  </si>
-  <si>
-    <t>jahati 1</t>
-  </si>
-  <si>
-    <t>sikkhati 2</t>
-  </si>
-  <si>
-    <t>paṭisevati 2</t>
-  </si>
-  <si>
-    <t>pavaḍḍhati 1</t>
-  </si>
-  <si>
-    <t>nikkhipati 3</t>
-  </si>
-  <si>
-    <t>bhajati 1</t>
-  </si>
-  <si>
-    <t>arahati 3</t>
-  </si>
-  <si>
-    <t>labhati</t>
-  </si>
-  <si>
-    <t>anussarati 1</t>
-  </si>
-  <si>
-    <t>nisīdati</t>
-  </si>
-  <si>
-    <t>bhavati 1</t>
-  </si>
-  <si>
-    <t>khādati</t>
-  </si>
-  <si>
-    <t>saṃvattati</t>
-  </si>
-  <si>
-    <t>gacchati 1</t>
-  </si>
-  <si>
-    <t>padahati 1</t>
-  </si>
-  <si>
-    <t>vāyamati</t>
-  </si>
-  <si>
-    <t>adhigacchati</t>
-  </si>
-  <si>
-    <t>abhiramati</t>
-  </si>
-  <si>
-    <t>pavisati</t>
-  </si>
-  <si>
-    <t>viharati 1</t>
-  </si>
-  <si>
-    <t>vaḍḍhati</t>
-  </si>
-  <si>
     <t>passati 1</t>
   </si>
   <si>
@@ -805,36 +805,36 @@
     <t>kassaka</t>
   </si>
   <si>
+    <t>samāpajjati 2</t>
+  </si>
+  <si>
+    <t>āpajjati 2</t>
+  </si>
+  <si>
+    <t>paṭipajjati 2</t>
+  </si>
+  <si>
+    <t>maññati 1</t>
+  </si>
+  <si>
+    <t>upādiyati</t>
+  </si>
+  <si>
+    <t>upapajjati 1</t>
+  </si>
+  <si>
+    <t>nibbindati 1</t>
+  </si>
+  <si>
+    <t>anuyuñjati 2</t>
+  </si>
+  <si>
+    <t>bhuñjati 1</t>
+  </si>
+  <si>
     <t>uppajjati 1</t>
   </si>
   <si>
-    <t>upapajjati 1</t>
-  </si>
-  <si>
-    <t>samāpajjati 2</t>
-  </si>
-  <si>
-    <t>āpajjati 2</t>
-  </si>
-  <si>
-    <t>paṭipajjati 2</t>
-  </si>
-  <si>
-    <t>maññati 1</t>
-  </si>
-  <si>
-    <t>upādiyati</t>
-  </si>
-  <si>
-    <t>nibbindati 1</t>
-  </si>
-  <si>
-    <t>anuyuñjati 2</t>
-  </si>
-  <si>
-    <t>bhuñjati 1</t>
-  </si>
-  <si>
     <t>jhāyati 2</t>
   </si>
   <si>
@@ -844,27 +844,27 @@
     <t>āpajjati 5</t>
   </si>
   <si>
+    <t>atthi 2</t>
+  </si>
+  <si>
+    <t>amha 1</t>
+  </si>
+  <si>
+    <t>asi 3</t>
+  </si>
+  <si>
+    <t>attha 12</t>
+  </si>
+  <si>
+    <t>amhi</t>
+  </si>
+  <si>
     <t>santi 3</t>
   </si>
   <si>
     <t>atthi 1</t>
   </si>
   <si>
-    <t>atthi 2</t>
-  </si>
-  <si>
-    <t>amha 1</t>
-  </si>
-  <si>
-    <t>asi 3</t>
-  </si>
-  <si>
-    <t>attha 12</t>
-  </si>
-  <si>
-    <t>amhi</t>
-  </si>
-  <si>
     <t>āmantesi</t>
   </si>
   <si>
@@ -916,15 +916,15 @@
     <t>muni 1</t>
   </si>
   <si>
+    <t>sāli</t>
+  </si>
+  <si>
+    <t>aggi</t>
+  </si>
+  <si>
     <t>gahapati</t>
   </si>
   <si>
-    <t>sāli</t>
-  </si>
-  <si>
-    <t>aggi</t>
-  </si>
-  <si>
     <t>isi</t>
   </si>
   <si>
@@ -973,54 +973,54 @@
     <t>āsi 1</t>
   </si>
   <si>
+    <t>mada 1</t>
+  </si>
+  <si>
+    <t>ājīva</t>
+  </si>
+  <si>
+    <t>appamāda</t>
+  </si>
+  <si>
+    <t>sambuddha 1</t>
+  </si>
+  <si>
+    <t>adhamma 2</t>
+  </si>
+  <si>
     <t>taca 1</t>
   </si>
   <si>
-    <t>mada 1</t>
-  </si>
-  <si>
-    <t>appamāda</t>
-  </si>
-  <si>
-    <t>ājīva</t>
-  </si>
-  <si>
-    <t>sambuddha 1</t>
-  </si>
-  <si>
-    <t>adhamma 2</t>
-  </si>
-  <si>
     <t>abhisamaya</t>
   </si>
   <si>
+    <t>mama 2</t>
+  </si>
+  <si>
+    <t>mayā 1</t>
+  </si>
+  <si>
+    <t>no 4</t>
+  </si>
+  <si>
+    <t>no 6</t>
+  </si>
+  <si>
+    <t>mayaṃ</t>
+  </si>
+  <si>
+    <t>me 5</t>
+  </si>
+  <si>
+    <t>no 7</t>
+  </si>
+  <si>
+    <t>amhākaṃ 3</t>
+  </si>
+  <si>
     <t>me 2</t>
   </si>
   <si>
-    <t>mama 2</t>
-  </si>
-  <si>
-    <t>mayā 1</t>
-  </si>
-  <si>
-    <t>no 4</t>
-  </si>
-  <si>
-    <t>no 6</t>
-  </si>
-  <si>
-    <t>mayaṃ</t>
-  </si>
-  <si>
-    <t>me 5</t>
-  </si>
-  <si>
-    <t>no 7</t>
-  </si>
-  <si>
-    <t>amhākaṃ 3</t>
-  </si>
-  <si>
     <t>ahaṃ</t>
   </si>
   <si>
@@ -1036,18 +1036,18 @@
     <t>neti 1</t>
   </si>
   <si>
+    <t>na 1</t>
+  </si>
+  <si>
+    <t>saddhiṃ</t>
+  </si>
+  <si>
+    <t>saha 2</t>
+  </si>
+  <si>
     <t>no 3</t>
   </si>
   <si>
-    <t>na 1</t>
-  </si>
-  <si>
-    <t>saddhiṃ</t>
-  </si>
-  <si>
-    <t>saha 2</t>
-  </si>
-  <si>
     <t>no 1</t>
   </si>
   <si>
@@ -1078,27 +1078,27 @@
     <t>dassati 1</t>
   </si>
   <si>
+    <t>vo 3</t>
+  </si>
+  <si>
+    <t>vo 2</t>
+  </si>
+  <si>
+    <t>tumhākaṃ 3</t>
+  </si>
+  <si>
+    <t>taṃ 3</t>
+  </si>
+  <si>
     <t>tumhākaṃ 2</t>
   </si>
   <si>
+    <t>tumhe 2</t>
+  </si>
+  <si>
     <t>tumhe 1</t>
   </si>
   <si>
-    <t>taṃ 3</t>
-  </si>
-  <si>
-    <t>vo 3</t>
-  </si>
-  <si>
-    <t>vo 2</t>
-  </si>
-  <si>
-    <t>tumhākaṃ 3</t>
-  </si>
-  <si>
-    <t>tumhe 2</t>
-  </si>
-  <si>
     <t>tvaṃ 1</t>
   </si>
   <si>
@@ -1153,12 +1153,12 @@
     <t>sakadāgāmī</t>
   </si>
   <si>
+    <t>sukhī 2</t>
+  </si>
+  <si>
     <t>brahmacārī 2</t>
   </si>
   <si>
-    <t>sukhī 2</t>
-  </si>
-  <si>
     <t>sabrahmacārī</t>
   </si>
   <si>
@@ -1171,30 +1171,30 @@
     <t>saṅgaha 1</t>
   </si>
   <si>
+    <t>paññavant</t>
+  </si>
+  <si>
+    <t>balavant</t>
+  </si>
+  <si>
+    <t>satimant 1</t>
+  </si>
+  <si>
     <t>sīlavant</t>
   </si>
   <si>
-    <t>paññavant</t>
-  </si>
-  <si>
-    <t>balavant</t>
-  </si>
-  <si>
-    <t>satimant 1</t>
-  </si>
-  <si>
     <t>assutavant</t>
   </si>
   <si>
+    <t>bhagavant 1</t>
+  </si>
+  <si>
+    <t>āyasmant 1</t>
+  </si>
+  <si>
     <t>cakkhumant 2</t>
   </si>
   <si>
-    <t>bhagavant 1</t>
-  </si>
-  <si>
-    <t>āyasmant 1</t>
-  </si>
-  <si>
     <t>satthar 1</t>
   </si>
   <si>
@@ -1219,12 +1219,12 @@
     <t>paricarati 3</t>
   </si>
   <si>
+    <t>kālena</t>
+  </si>
+  <si>
     <t>vā 1</t>
   </si>
   <si>
-    <t>kālena</t>
-  </si>
-  <si>
     <t>yadā</t>
   </si>
   <si>
@@ -1288,24 +1288,24 @@
     <t>nahāyati</t>
   </si>
   <si>
+    <t>gaccheyya</t>
+  </si>
+  <si>
+    <t>jāneyya</t>
+  </si>
+  <si>
+    <t>āgaccheyya</t>
+  </si>
+  <si>
+    <t>vadeyya</t>
+  </si>
+  <si>
+    <t>adhigaccheyya</t>
+  </si>
+  <si>
     <t>passeyya 1</t>
   </si>
   <si>
-    <t>gaccheyya</t>
-  </si>
-  <si>
-    <t>jāneyya</t>
-  </si>
-  <si>
-    <t>āgaccheyya</t>
-  </si>
-  <si>
-    <t>vadeyya</t>
-  </si>
-  <si>
-    <t>adhigaccheyya</t>
-  </si>
-  <si>
     <t>uppajjeyya</t>
   </si>
   <si>
@@ -1324,63 +1324,63 @@
     <t>assa 3</t>
   </si>
   <si>
+    <t>sikkhā 2</t>
+  </si>
+  <si>
+    <t>gāthā 1</t>
+  </si>
+  <si>
+    <t>jarā</t>
+  </si>
+  <si>
+    <t>vīmaṃsā 1</t>
+  </si>
+  <si>
+    <t>disā 1</t>
+  </si>
+  <si>
+    <t>paññā 1</t>
+  </si>
+  <si>
+    <t>abhijjhā</t>
+  </si>
+  <si>
+    <t>senā</t>
+  </si>
+  <si>
+    <t>sākhā 1</t>
+  </si>
+  <si>
+    <t>bāhā 1</t>
+  </si>
+  <si>
+    <t>desanā 3</t>
+  </si>
+  <si>
+    <t>vācā 1</t>
+  </si>
+  <si>
+    <t>taṇhā 1</t>
+  </si>
+  <si>
+    <t>vedanā 1</t>
+  </si>
+  <si>
+    <t>jivhā</t>
+  </si>
+  <si>
+    <t>upāsikā</t>
+  </si>
+  <si>
+    <t>pabbajjā</t>
+  </si>
+  <si>
+    <t>devatā</t>
+  </si>
+  <si>
     <t>sacchikiriyā</t>
   </si>
   <si>
-    <t>pabbajjā</t>
-  </si>
-  <si>
-    <t>sikkhā 2</t>
-  </si>
-  <si>
-    <t>gāthā 1</t>
-  </si>
-  <si>
-    <t>jarā</t>
-  </si>
-  <si>
-    <t>vīmaṃsā 1</t>
-  </si>
-  <si>
-    <t>disā 1</t>
-  </si>
-  <si>
-    <t>paññā 1</t>
-  </si>
-  <si>
-    <t>abhijjhā</t>
-  </si>
-  <si>
-    <t>senā</t>
-  </si>
-  <si>
-    <t>sākhā 1</t>
-  </si>
-  <si>
-    <t>bāhā 1</t>
-  </si>
-  <si>
-    <t>desanā 3</t>
-  </si>
-  <si>
-    <t>vācā 1</t>
-  </si>
-  <si>
-    <t>taṇhā 1</t>
-  </si>
-  <si>
-    <t>vedanā 1</t>
-  </si>
-  <si>
-    <t>jivhā</t>
-  </si>
-  <si>
-    <t>upāsikā</t>
-  </si>
-  <si>
-    <t>devatā</t>
-  </si>
-  <si>
     <t>pajā 2</t>
   </si>
   <si>
@@ -1471,12 +1471,12 @@
     <t>dhītar</t>
   </si>
   <si>
+    <t>āgamma 1</t>
+  </si>
+  <si>
     <t>samādāya 2</t>
   </si>
   <si>
-    <t>āgamma 1</t>
-  </si>
-  <si>
     <t>vineyya 1</t>
   </si>
   <si>
@@ -1498,33 +1498,33 @@
     <t>nisajja</t>
   </si>
   <si>
+    <t>ṭhiti 1</t>
+  </si>
+  <si>
+    <t>kuṭi 1</t>
+  </si>
+  <si>
+    <t>visuddhi 1</t>
+  </si>
+  <si>
+    <t>āpatti 2</t>
+  </si>
+  <si>
     <t>diṭṭhi 1</t>
   </si>
   <si>
+    <t>samāpatti 1</t>
+  </si>
+  <si>
+    <t>ruci</t>
+  </si>
+  <si>
+    <t>sugati</t>
+  </si>
+  <si>
     <t>sati 2</t>
   </si>
   <si>
-    <t>ṭhiti 1</t>
-  </si>
-  <si>
-    <t>kuṭi 1</t>
-  </si>
-  <si>
-    <t>visuddhi 1</t>
-  </si>
-  <si>
-    <t>āpatti 2</t>
-  </si>
-  <si>
-    <t>samāpatti 1</t>
-  </si>
-  <si>
-    <t>ruci</t>
-  </si>
-  <si>
-    <t>sugati</t>
-  </si>
-  <si>
     <t>pīti 1</t>
   </si>
   <si>
@@ -1555,12 +1555,12 @@
     <t>ekato 1</t>
   </si>
   <si>
+    <t>sabbattha 1</t>
+  </si>
+  <si>
     <t>kuto 1</t>
   </si>
   <si>
-    <t>sabbattha 1</t>
-  </si>
-  <si>
     <t>tattha 1</t>
   </si>
   <si>
@@ -1612,129 +1612,129 @@
     <t>piṇḍāya</t>
   </si>
   <si>
+    <t>bhūta 3</t>
+  </si>
+  <si>
+    <t>indriya 1</t>
+  </si>
+  <si>
+    <t>sukhāya</t>
+  </si>
+  <si>
+    <t>hitāya</t>
+  </si>
+  <si>
+    <t>rūpa 1</t>
+  </si>
+  <si>
+    <t>anagāriya</t>
+  </si>
+  <si>
+    <t>agāra 2</t>
+  </si>
+  <si>
+    <t>sukha 2</t>
+  </si>
+  <si>
+    <t>hita 3</t>
+  </si>
+  <si>
+    <t>nāma 5</t>
+  </si>
+  <si>
+    <t>vīriya 1</t>
+  </si>
+  <si>
+    <t>vepulla 1</t>
+  </si>
+  <si>
+    <t>maraṇa</t>
+  </si>
+  <si>
+    <t>nidāna 1</t>
+  </si>
+  <si>
+    <t>kula 1</t>
+  </si>
+  <si>
+    <t>pāmojja</t>
+  </si>
+  <si>
+    <t>arañña</t>
+  </si>
+  <si>
+    <t>bala 2</t>
+  </si>
+  <si>
+    <t>pamāṇa 3</t>
+  </si>
+  <si>
+    <t>upādāna 2</t>
+  </si>
+  <si>
+    <t>sarīra 1</t>
+  </si>
+  <si>
+    <t>passa 1</t>
+  </si>
+  <si>
+    <t>vattha 1</t>
+  </si>
+  <si>
+    <t>puñña 1</t>
+  </si>
+  <si>
+    <t>agāra 1</t>
+  </si>
+  <si>
+    <t>dassanāya 2</t>
+  </si>
+  <si>
+    <t>itthatta 1</t>
+  </si>
+  <si>
+    <t>mūla 2</t>
+  </si>
+  <si>
+    <t>domanassa</t>
+  </si>
+  <si>
+    <t>dukkha 3</t>
+  </si>
+  <si>
+    <t>bhesajja</t>
+  </si>
+  <si>
+    <t>aparihāna</t>
+  </si>
+  <si>
+    <t>bhāsita 1</t>
+  </si>
+  <si>
+    <t>nibbāna 2</t>
+  </si>
+  <si>
+    <t>saraṇa 2</t>
+  </si>
+  <si>
+    <t>vajja 3</t>
+  </si>
+  <si>
+    <t>sikkhāpada</t>
+  </si>
+  <si>
+    <t>bhaya 3</t>
+  </si>
+  <si>
+    <t>bhojana 2</t>
+  </si>
+  <si>
     <t>adinna 1</t>
   </si>
   <si>
-    <t>sikkhāpada</t>
-  </si>
-  <si>
-    <t>bhaya 3</t>
-  </si>
-  <si>
     <t>rūpa 3</t>
   </si>
   <si>
-    <t>bhūta 3</t>
-  </si>
-  <si>
-    <t>indriya 1</t>
-  </si>
-  <si>
-    <t>sukhāya</t>
-  </si>
-  <si>
-    <t>hitāya</t>
-  </si>
-  <si>
-    <t>rūpa 1</t>
-  </si>
-  <si>
-    <t>anagāriya</t>
-  </si>
-  <si>
-    <t>agāra 2</t>
-  </si>
-  <si>
-    <t>sukha 2</t>
-  </si>
-  <si>
-    <t>hita 3</t>
-  </si>
-  <si>
-    <t>nāma 5</t>
-  </si>
-  <si>
-    <t>vīriya 1</t>
-  </si>
-  <si>
-    <t>vepulla 1</t>
-  </si>
-  <si>
-    <t>maraṇa</t>
-  </si>
-  <si>
-    <t>nidāna 1</t>
-  </si>
-  <si>
-    <t>kula 1</t>
-  </si>
-  <si>
-    <t>pāmojja</t>
-  </si>
-  <si>
-    <t>bala 2</t>
-  </si>
-  <si>
-    <t>arañña</t>
-  </si>
-  <si>
-    <t>pamāṇa 3</t>
-  </si>
-  <si>
-    <t>upādāna 2</t>
-  </si>
-  <si>
-    <t>sarīra 1</t>
-  </si>
-  <si>
-    <t>passa 1</t>
-  </si>
-  <si>
-    <t>vattha 1</t>
-  </si>
-  <si>
-    <t>puñña 1</t>
-  </si>
-  <si>
-    <t>agāra 1</t>
-  </si>
-  <si>
-    <t>dassanāya 2</t>
-  </si>
-  <si>
-    <t>itthatta 1</t>
-  </si>
-  <si>
-    <t>mūla 2</t>
-  </si>
-  <si>
-    <t>domanassa</t>
-  </si>
-  <si>
-    <t>dukkha 3</t>
-  </si>
-  <si>
-    <t>bhesajja</t>
-  </si>
-  <si>
-    <t>aparihāna</t>
-  </si>
-  <si>
-    <t>bhāsita 1</t>
-  </si>
-  <si>
-    <t>nibbāna 2</t>
-  </si>
-  <si>
-    <t>saraṇa 2</t>
-  </si>
-  <si>
-    <t>vajja 3</t>
-  </si>
-  <si>
-    <t>bhojana 2</t>
-  </si>
-  <si>
     <t>viññāṇa 1</t>
   </si>
   <si>
@@ -1825,36 +1825,36 @@
     <t>aṭṭhi 1</t>
   </si>
   <si>
+    <t>tāva 1</t>
+  </si>
+  <si>
+    <t>api 7</t>
+  </si>
+  <si>
     <t>nu</t>
   </si>
   <si>
     <t>kallaṃ</t>
   </si>
   <si>
+    <t>alaṃ 2</t>
+  </si>
+  <si>
+    <t>kathaṃ 1</t>
+  </si>
+  <si>
+    <t>alaṃ 3</t>
+  </si>
+  <si>
+    <t>yāva 1</t>
+  </si>
+  <si>
+    <t>sakkā 1</t>
+  </si>
+  <si>
     <t>alaṃ 1</t>
   </si>
   <si>
-    <t>tāva 1</t>
-  </si>
-  <si>
-    <t>api 7</t>
-  </si>
-  <si>
-    <t>alaṃ 2</t>
-  </si>
-  <si>
-    <t>kathaṃ 1</t>
-  </si>
-  <si>
-    <t>alaṃ 3</t>
-  </si>
-  <si>
-    <t>yāva 1</t>
-  </si>
-  <si>
-    <t>sakkā 1</t>
-  </si>
-  <si>
     <t>alaṃ 5</t>
   </si>
   <si>
@@ -1945,24 +1945,24 @@
     <t>that; such (person or place or thing); so and so</t>
   </si>
   <si>
+    <t>not asking permission; not informing</t>
+  </si>
+  <si>
+    <t>seeing</t>
+  </si>
+  <si>
+    <t>knowing</t>
+  </si>
+  <si>
+    <t>seeing; regarding; considering</t>
+  </si>
+  <si>
+    <t>standing; standing still</t>
+  </si>
+  <si>
     <t>remembering; recollecting</t>
   </si>
   <si>
-    <t>not asking permission; not informing</t>
-  </si>
-  <si>
-    <t>seeing</t>
-  </si>
-  <si>
-    <t>knowing</t>
-  </si>
-  <si>
-    <t>seeing; regarding; considering</t>
-  </si>
-  <si>
-    <t>standing; standing still</t>
-  </si>
-  <si>
     <t>going; walking; travelling</t>
   </si>
   <si>
@@ -1993,27 +1993,297 @@
     <t>wishing (for); desiring (for); seeking (for)</t>
   </si>
   <si>
+    <t>discipline; training; lit. leading out</t>
+  </si>
+  <si>
+    <t>teaching; doctrine</t>
+  </si>
+  <si>
+    <t>way; nature; habit; property; quality; lit. going around</t>
+  </si>
+  <si>
+    <t>human; human being; man</t>
+  </si>
+  <si>
+    <t>deity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">various opinions; proliferation; endless conceptualization; lit. expanding; spreading </t>
+  </si>
+  <si>
+    <t>offence requiring suspension; lit. offence requiring involvement of the community from start to finish</t>
+  </si>
+  <si>
+    <t>control; authority; power; mastery</t>
+  </si>
+  <si>
+    <t>calf; yearling; young animal</t>
+  </si>
+  <si>
+    <t>an individual; a person</t>
+  </si>
+  <si>
+    <t>home (of); dwelling (of); abode (of)</t>
+  </si>
+  <si>
+    <t>nature; character</t>
+  </si>
+  <si>
+    <t>full moon or new moon observance day</t>
+  </si>
+  <si>
+    <t>being; existence; becoming</t>
+  </si>
+  <si>
+    <t>rainy season; monsoon</t>
+  </si>
+  <si>
+    <t>house; dwelling place; residence</t>
+  </si>
+  <si>
+    <t>obstacle; danger; lit. coming in-between</t>
+  </si>
+  <si>
+    <t>name of one of the Buddha's chief disciples; great disciple of the Buddha; foremost disciple in psychic power; lit. descendent of Muggala</t>
+  </si>
+  <si>
     <t>act; practice; behaviour</t>
   </si>
   <si>
+    <t>control (over); restraint (of); holding back (of)</t>
+  </si>
+  <si>
+    <t>road; path; track</t>
+  </si>
+  <si>
+    <t>child; son</t>
+  </si>
+  <si>
+    <t>bean</t>
+  </si>
+  <si>
+    <t>wealth; possession; property</t>
+  </si>
+  <si>
+    <t>cause; reason; supporting condition; precondition; requirement</t>
+  </si>
+  <si>
+    <t>man; person</t>
+  </si>
+  <si>
+    <t>time; occasion; lit. coming together; meeting</t>
+  </si>
+  <si>
+    <t>meaning; significance</t>
+  </si>
+  <si>
+    <t>name of one of the Buddha's chief disciples; great disciple of the Buddha; foremost disciple in great wisdom; lit. son of Sāri</t>
+  </si>
+  <si>
+    <t>question; enquiry</t>
+  </si>
+  <si>
+    <t>disease; sickness; illness; affliction</t>
+  </si>
+  <si>
+    <t>mental formation; mental activity; thought processes; fourth of the five aggregates; lit. making together</t>
+  </si>
+  <si>
     <t>man of the ruling caste; high caste man; nobleman</t>
   </si>
   <si>
+    <t>touch; contact; sense impingement</t>
+  </si>
+  <si>
+    <t>common man; ordinary man; normal person; man in the street; lit. individual person</t>
+  </si>
+  <si>
+    <t>stick; truncheon; nightstick; club</t>
+  </si>
+  <si>
     <t>way; means; method; lit. path</t>
   </si>
   <si>
     <t>matter; thing; phenomena</t>
   </si>
   <si>
+    <t>taste; flavour</t>
+  </si>
+  <si>
+    <t>young man; young gentleman; young Brahman; man</t>
+  </si>
+  <si>
     <t>world; universe; cosmos</t>
   </si>
   <si>
     <t>sense desire (of); sensual pleasure (of)</t>
   </si>
   <si>
+    <t>watch (of the night); 1/3 of a night; lit. restraint</t>
+  </si>
+  <si>
+    <t>leg; foot</t>
+  </si>
+  <si>
+    <t>schism; break; split</t>
+  </si>
+  <si>
+    <t>requisite; accessory</t>
+  </si>
+  <si>
+    <t>range; mode; way</t>
+  </si>
+  <si>
+    <t>personal name of the Buddha's attendant; great disciple of the Buddha; foremost disciple in great learning, remembrance, conduct, resoluteness and service; lit. happy</t>
+  </si>
+  <si>
+    <t>benefit; profit; good; welfare; goal</t>
+  </si>
+  <si>
+    <t>profit; benefit; advantage</t>
+  </si>
+  <si>
+    <t>the wind; air</t>
+  </si>
+  <si>
+    <t>bird</t>
+  </si>
+  <si>
+    <t>sage; intelligent person; wise man</t>
+  </si>
+  <si>
+    <t>hand</t>
+  </si>
+  <si>
+    <t>a living being; creature; sentient beings</t>
+  </si>
+  <si>
+    <t>hell; lit. no good fortune</t>
+  </si>
+  <si>
+    <t>state of suffering; lit. bad fall</t>
+  </si>
+  <si>
+    <t>pride; conceit; comparison</t>
+  </si>
+  <si>
+    <t>group; host; multitude; lit. collection</t>
+  </si>
+  <si>
+    <t>community; assembly of monks</t>
+  </si>
+  <si>
+    <t>well; lit. water drinking</t>
+  </si>
+  <si>
+    <t>affliction; agitation; trouble; despair</t>
+  </si>
+  <si>
+    <t>lamentation; wailing; crying</t>
+  </si>
+  <si>
+    <t>grief; sorrow</t>
+  </si>
+  <si>
+    <t>anger; hatred; ill-will</t>
+  </si>
+  <si>
+    <t>desire; lust; passion; attachment</t>
+  </si>
+  <si>
+    <t>breaking-up (of); breaking apart (of); death</t>
+  </si>
+  <si>
     <t>disciple; pupil; lit. hearer</t>
   </si>
   <si>
+    <t>support; requisite; necessity</t>
+  </si>
+  <si>
+    <t>excrement; dung; faeces</t>
+  </si>
+  <si>
+    <t>urine; lit. flowing out</t>
+  </si>
+  <si>
+    <t>wearing away (of); exhaustion (of); erosion (of); depletion (of); slow destruction (of)</t>
+  </si>
+  <si>
+    <t>discharge; suppuration; outflow; effluent; (comm) impurity</t>
+  </si>
+  <si>
+    <t>obstacle; hindrance; obstruction; barrier</t>
+  </si>
+  <si>
+    <t>trainee; belonging to training; one who is in the course of perfection</t>
+  </si>
+  <si>
+    <t>quality; characteristic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stilling (of); serenity (of); calming (of); settling (of); peace (of); (comm) mental unification </t>
+  </si>
+  <si>
+    <t>cross-legged sitting position</t>
+  </si>
+  <si>
+    <t>independence; freedom from clinging; non-attachment</t>
+  </si>
+  <si>
+    <t>giving up; relinquishing; dropping; abandoning</t>
+  </si>
+  <si>
+    <t>abandoning; giving up; renunciation</t>
+  </si>
+  <si>
+    <t>clarity; light; brightness</t>
+  </si>
+  <si>
+    <t>name of a monk; Buddha's son</t>
+  </si>
+  <si>
+    <t>smell; scent; odour</t>
+  </si>
+  <si>
+    <t>family name of the Buddha; lit. of the Gotama clan</t>
+  </si>
+  <si>
+    <t>ascetic; renunciant; holy man; monk; recluse; lit. who makes an effort; calm one</t>
+  </si>
+  <si>
+    <t>ending; termination; cessation; finishing</t>
+  </si>
+  <si>
+    <t>fading of desire (for); dispassion (towards); detachment (from); indifference (to)</t>
+  </si>
+  <si>
+    <t>arising; origin; appearance; lit. come up together</t>
+  </si>
+  <si>
+    <t>mass; heap; pile</t>
+  </si>
+  <si>
+    <t>enlightenment; full awakening; perfect understanding</t>
+  </si>
+  <si>
+    <t>calmness; peace; tranquillity</t>
+  </si>
+  <si>
+    <t>carelessness; negligence; heedlessness</t>
+  </si>
+  <si>
+    <t>death; Death personified; the Evil One; Māra</t>
+  </si>
+  <si>
+    <t>Brahman; priest; man of the Brahman caste</t>
+  </si>
+  <si>
+    <t>(of water) flood; deluge; torrent</t>
+  </si>
+  <si>
+    <t>Sakyan; of the Sakyan people</t>
+  </si>
+  <si>
     <t>arrival (at); attainment (of); reaching (of)</t>
   </si>
   <si>
@@ -2023,6 +2293,48 @@
     <t>surpassing; overcoming; going beyond</t>
   </si>
   <si>
+    <t>control (according to); restraint (according to); holding back (according to)</t>
+  </si>
+  <si>
+    <t>non-attention; ignoring; lit. not making in mind</t>
+  </si>
+  <si>
+    <t>proposition; synopsis; statement in brief; summary; introduction</t>
+  </si>
+  <si>
+    <t>(vinaya) consent; agreement; approval</t>
+  </si>
+  <si>
+    <t>aggregate; combination; conglomeration</t>
+  </si>
+  <si>
+    <t>arahant; saint; holy man; sage</t>
+  </si>
+  <si>
+    <t>stream; river; current</t>
+  </si>
+  <si>
+    <t>calming (of); subsiding (of); settling (of); peace (of)</t>
+  </si>
+  <si>
+    <t>world; plane of existence</t>
+  </si>
+  <si>
+    <t>the sea; ocean</t>
+  </si>
+  <si>
+    <t>demon; malevolent being; enemy of the devas; lit. anti-hero</t>
+  </si>
+  <si>
+    <t>intention; volitional formation; karmic activity; lit. making together</t>
+  </si>
+  <si>
+    <t>waning; fading away; lit. discolouring</t>
+  </si>
+  <si>
+    <t>food; fuel; sustenance</t>
+  </si>
+  <si>
     <t>distinction; attainment</t>
   </si>
   <si>
@@ -2035,318 +2347,6 @@
     <t>hair of the head</t>
   </si>
   <si>
-    <t>discipline; training; lit. leading out</t>
-  </si>
-  <si>
-    <t>teaching; doctrine</t>
-  </si>
-  <si>
-    <t>way; nature; habit; property; quality; lit. going around</t>
-  </si>
-  <si>
-    <t>human; human being; man</t>
-  </si>
-  <si>
-    <t>deity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">various opinions; proliferation; endless conceptualization; lit. expanding; spreading </t>
-  </si>
-  <si>
-    <t>offence requiring suspension; lit. offence requiring involvement of the community from start to finish</t>
-  </si>
-  <si>
-    <t>control; authority; power; mastery</t>
-  </si>
-  <si>
-    <t>calf; yearling; young animal</t>
-  </si>
-  <si>
-    <t>an individual; a person</t>
-  </si>
-  <si>
-    <t>home (of); dwelling (of); abode (of)</t>
-  </si>
-  <si>
-    <t>nature; character</t>
-  </si>
-  <si>
-    <t>full moon or new moon observance day</t>
-  </si>
-  <si>
-    <t>being; existence; becoming</t>
-  </si>
-  <si>
-    <t>rainy season; monsoon</t>
-  </si>
-  <si>
-    <t>house; dwelling place; residence</t>
-  </si>
-  <si>
-    <t>obstacle; danger; lit. coming in-between</t>
-  </si>
-  <si>
-    <t>name of one of the Buddha's chief disciples; great disciple of the Buddha; foremost disciple in psychic power; lit. descendent of Muggala</t>
-  </si>
-  <si>
-    <t>control (over); restraint (of); holding back (of)</t>
-  </si>
-  <si>
-    <t>bean</t>
-  </si>
-  <si>
-    <t>road; path; track</t>
-  </si>
-  <si>
-    <t>child; son</t>
-  </si>
-  <si>
-    <t>wealth; possession; property</t>
-  </si>
-  <si>
-    <t>cause; reason; supporting condition; precondition; requirement</t>
-  </si>
-  <si>
-    <t>time; occasion; lit. coming together; meeting</t>
-  </si>
-  <si>
-    <t>man; person</t>
-  </si>
-  <si>
-    <t>meaning; significance</t>
-  </si>
-  <si>
-    <t>name of one of the Buddha's chief disciples; great disciple of the Buddha; foremost disciple in great wisdom; lit. son of Sāri</t>
-  </si>
-  <si>
-    <t>question; enquiry</t>
-  </si>
-  <si>
-    <t>disease; sickness; illness; affliction</t>
-  </si>
-  <si>
-    <t>mental formation; mental activity; thought processes; fourth of the five aggregates; lit. making together</t>
-  </si>
-  <si>
-    <t>touch; contact; sense impingement</t>
-  </si>
-  <si>
-    <t>common man; ordinary man; normal person; man in the street; lit. individual person</t>
-  </si>
-  <si>
-    <t>stick; truncheon; nightstick; club</t>
-  </si>
-  <si>
-    <t>taste; flavour</t>
-  </si>
-  <si>
-    <t>young man; young gentleman; young Brahman; man</t>
-  </si>
-  <si>
-    <t>watch (of the night); 1/3 of a night; lit. restraint</t>
-  </si>
-  <si>
-    <t>leg; foot</t>
-  </si>
-  <si>
-    <t>schism; break; split</t>
-  </si>
-  <si>
-    <t>requisite; accessory</t>
-  </si>
-  <si>
-    <t>range; mode; way</t>
-  </si>
-  <si>
-    <t>personal name of the Buddha's attendant; great disciple of the Buddha; foremost disciple in great learning, remembrance, conduct, resoluteness and service; lit. happy</t>
-  </si>
-  <si>
-    <t>benefit; profit; good; welfare; goal</t>
-  </si>
-  <si>
-    <t>profit; benefit; advantage</t>
-  </si>
-  <si>
-    <t>the wind; air</t>
-  </si>
-  <si>
-    <t>bird</t>
-  </si>
-  <si>
-    <t>sage; intelligent person; wise man</t>
-  </si>
-  <si>
-    <t>hand</t>
-  </si>
-  <si>
-    <t>a living being; creature; sentient beings</t>
-  </si>
-  <si>
-    <t>hell; lit. no good fortune</t>
-  </si>
-  <si>
-    <t>state of suffering; lit. bad fall</t>
-  </si>
-  <si>
-    <t>pride; conceit; comparison</t>
-  </si>
-  <si>
-    <t>group; host; multitude; lit. collection</t>
-  </si>
-  <si>
-    <t>community; assembly of monks</t>
-  </si>
-  <si>
-    <t>well; lit. water drinking</t>
-  </si>
-  <si>
-    <t>affliction; agitation; trouble; despair</t>
-  </si>
-  <si>
-    <t>lamentation; wailing; crying</t>
-  </si>
-  <si>
-    <t>grief; sorrow</t>
-  </si>
-  <si>
-    <t>anger; hatred; ill-will</t>
-  </si>
-  <si>
-    <t>desire; lust; passion; attachment</t>
-  </si>
-  <si>
-    <t>breaking-up (of); breaking apart (of); death</t>
-  </si>
-  <si>
-    <t>support; requisite; necessity</t>
-  </si>
-  <si>
-    <t>excrement; dung; faeces</t>
-  </si>
-  <si>
-    <t>urine; lit. flowing out</t>
-  </si>
-  <si>
-    <t>wearing away (of); exhaustion (of); erosion (of); depletion (of); slow destruction (of)</t>
-  </si>
-  <si>
-    <t>discharge; suppuration; outflow; effluent; (comm) impurity</t>
-  </si>
-  <si>
-    <t>obstacle; hindrance; obstruction; barrier</t>
-  </si>
-  <si>
-    <t>trainee; belonging to training; one who is in the course of perfection</t>
-  </si>
-  <si>
-    <t>quality; characteristic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stilling (of); serenity (of); calming (of); settling (of); peace (of); (comm) mental unification </t>
-  </si>
-  <si>
-    <t>cross-legged sitting position</t>
-  </si>
-  <si>
-    <t>independence; freedom from clinging; non-attachment</t>
-  </si>
-  <si>
-    <t>giving up; relinquishing; dropping; abandoning</t>
-  </si>
-  <si>
-    <t>abandoning; giving up; renunciation</t>
-  </si>
-  <si>
-    <t>clarity; light; brightness</t>
-  </si>
-  <si>
-    <t>name of a monk; Buddha's son</t>
-  </si>
-  <si>
-    <t>smell; scent; odour</t>
-  </si>
-  <si>
-    <t>arising; origin; appearance; lit. come up together</t>
-  </si>
-  <si>
-    <t>mass; heap; pile</t>
-  </si>
-  <si>
-    <t>family name of the Buddha; lit. of the Gotama clan</t>
-  </si>
-  <si>
-    <t>ascetic; renunciant; holy man; monk; recluse; lit. who makes an effort; calm one</t>
-  </si>
-  <si>
-    <t>ending; termination; cessation; finishing</t>
-  </si>
-  <si>
-    <t>fading of desire (for); dispassion (towards); detachment (from); indifference (to)</t>
-  </si>
-  <si>
-    <t>enlightenment; full awakening; perfect understanding</t>
-  </si>
-  <si>
-    <t>calmness; peace; tranquillity</t>
-  </si>
-  <si>
-    <t>carelessness; negligence; heedlessness</t>
-  </si>
-  <si>
-    <t>death; Death personified; the Evil One; Māra</t>
-  </si>
-  <si>
-    <t>Brahman; priest; man of the Brahman caste</t>
-  </si>
-  <si>
-    <t>(of water) flood; deluge; torrent</t>
-  </si>
-  <si>
-    <t>Sakyan; of the Sakyan people</t>
-  </si>
-  <si>
-    <t>control (according to); restraint (according to); holding back (according to)</t>
-  </si>
-  <si>
-    <t>non-attention; ignoring; lit. not making in mind</t>
-  </si>
-  <si>
-    <t>proposition; synopsis; statement in brief; summary; introduction</t>
-  </si>
-  <si>
-    <t>(vinaya) consent; agreement; approval</t>
-  </si>
-  <si>
-    <t>aggregate; combination; conglomeration</t>
-  </si>
-  <si>
-    <t>arahant; saint; holy man; sage</t>
-  </si>
-  <si>
-    <t>stream; river; current</t>
-  </si>
-  <si>
-    <t>calming (of); subsiding (of); settling (of); peace (of)</t>
-  </si>
-  <si>
-    <t>world; plane of existence</t>
-  </si>
-  <si>
-    <t>the sea; ocean</t>
-  </si>
-  <si>
-    <t>demon; malevolent being; enemy of the devas; lit. anti-hero</t>
-  </si>
-  <si>
-    <t>intention; volitional formation; karmic activity; lit. making together</t>
-  </si>
-  <si>
-    <t>waning; fading away; lit. discolouring</t>
-  </si>
-  <si>
-    <t>food; fuel; sustenance</t>
-  </si>
-  <si>
     <t>friend; companion; fellow traveller</t>
   </si>
   <si>
@@ -2467,165 +2467,165 @@
     <t>name of the people of Kosala; Kosalans</t>
   </si>
   <si>
+    <t>appearing again; renewed existence; rebirth; further becoming</t>
+  </si>
+  <si>
     <t>(vinaya) 227 precepts for Buddhist monks</t>
   </si>
   <si>
-    <t>appearing again; renewed existence; rebirth; further becoming</t>
-  </si>
-  <si>
     <t>analysis; classification; breakdown</t>
   </si>
   <si>
+    <t>gives up; renounces; forsakes; abandons; let go</t>
+  </si>
+  <si>
+    <t>practices; indulges (in); engages (in); lit. associates</t>
+  </si>
+  <si>
+    <t>removes; takes away; packs up</t>
+  </si>
+  <si>
+    <t>binds; ties up; imprisons</t>
+  </si>
+  <si>
+    <t>see! look! watch!</t>
+  </si>
+  <si>
+    <t>lasts; remains; persists; lit. stands</t>
+  </si>
+  <si>
+    <t>increases more and more; surpasses; outgrows</t>
+  </si>
+  <si>
+    <t>says (to); speaks (to); tells (to)</t>
+  </si>
+  <si>
+    <t>goes forth; ordains as monk; renounces the household life</t>
+  </si>
+  <si>
+    <t>recites</t>
+  </si>
+  <si>
     <t>goes; goes away (from); leaves</t>
   </si>
   <si>
+    <t>begins; starts; arouses</t>
+  </si>
+  <si>
+    <t>wishes; desires</t>
+  </si>
+  <si>
+    <t>wards off; prevents; guards against</t>
+  </si>
+  <si>
+    <t>approaches; goes (to); visits</t>
+  </si>
+  <si>
+    <t>says; speaks</t>
+  </si>
+  <si>
+    <t>asks (for); begs (for) requests</t>
+  </si>
+  <si>
+    <t>takes; steals; robs</t>
+  </si>
+  <si>
+    <t>obtains; receives; gets</t>
+  </si>
+  <si>
+    <t>exhales; breathes out</t>
+  </si>
+  <si>
+    <t>breathes; inhales</t>
+  </si>
+  <si>
+    <t>wishes (for); desires; intends; plans</t>
+  </si>
+  <si>
+    <t>grabs hold (of); seizes; takes</t>
+  </si>
+  <si>
     <t>speaks; says; proclaims</t>
   </si>
   <si>
+    <t>advises; instructs; admonishes</t>
+  </si>
+  <si>
+    <t>understands; gets; lit. sees</t>
+  </si>
+  <si>
+    <t>leaves; abandons; gives up; forsakes</t>
+  </si>
+  <si>
+    <t>trains (in); trains (for the purpose of); practices (for the sake of); practice (to); lit. trains</t>
+  </si>
+  <si>
+    <t>uses; makes use (of); lit. associates</t>
+  </si>
+  <si>
+    <t>grows; increases</t>
+  </si>
+  <si>
+    <t>sets aside; lays aside; keeps; stores; saves; lit. throws down</t>
+  </si>
+  <si>
+    <t>associates (with); keeps company (with)</t>
+  </si>
+  <si>
+    <t>should; ought (to); is suitable (for); it is befitting (for)</t>
+  </si>
+  <si>
     <t>proceeds; continues; goes forward; practices</t>
   </si>
   <si>
+    <t>gets; receives; obtains</t>
+  </si>
+  <si>
+    <t>remembers; recollects</t>
+  </si>
+  <si>
+    <t>sits; sits down</t>
+  </si>
+  <si>
+    <t>is; is being; becomes; exists</t>
+  </si>
+  <si>
+    <t>eats; chews; bites</t>
+  </si>
+  <si>
     <t>asks; enquires; questions</t>
   </si>
   <si>
+    <t>leads (to); is useful (for); is conducive to</t>
+  </si>
+  <si>
+    <t>goes; walks; moves; wanders around</t>
+  </si>
+  <si>
+    <t>exerts oneself; strives; applies oneself; lit. puts forward</t>
+  </si>
+  <si>
+    <t>tries; makes an effort; strives for; exerts oneself</t>
+  </si>
+  <si>
+    <t>gets to; attains; finds; acquires; obtains; lit. goes up to</t>
+  </si>
+  <si>
+    <t>enjoys; finds high pleasure in</t>
+  </si>
+  <si>
+    <t>enters; goes into</t>
+  </si>
+  <si>
+    <t>lives (in); dwells (in)</t>
+  </si>
+  <si>
+    <t>grows; increases; multiplies</t>
+  </si>
+  <si>
     <t>it is suitable (for); it is proper (for); it is fitting (for); it is allowable</t>
   </si>
   <si>
-    <t>gives up; renounces; forsakes; abandons; let go</t>
-  </si>
-  <si>
-    <t>practices; indulges (in); engages (in); lit. associates</t>
-  </si>
-  <si>
-    <t>removes; takes away; packs up</t>
-  </si>
-  <si>
-    <t>binds; ties up; imprisons</t>
-  </si>
-  <si>
-    <t>see! look! watch!</t>
-  </si>
-  <si>
-    <t>lasts; remains; persists; lit. stands</t>
-  </si>
-  <si>
-    <t>goes forth; ordains as monk; renounces the household life</t>
-  </si>
-  <si>
-    <t>increases more and more; surpasses; outgrows</t>
-  </si>
-  <si>
-    <t>says (to); speaks (to); tells (to)</t>
-  </si>
-  <si>
-    <t>recites</t>
-  </si>
-  <si>
-    <t>begins; starts; arouses</t>
-  </si>
-  <si>
-    <t>wishes; desires</t>
-  </si>
-  <si>
-    <t>wards off; prevents; guards against</t>
-  </si>
-  <si>
-    <t>approaches; goes (to); visits</t>
-  </si>
-  <si>
-    <t>says; speaks</t>
-  </si>
-  <si>
-    <t>asks (for); begs (for) requests</t>
-  </si>
-  <si>
-    <t>takes; steals; robs</t>
-  </si>
-  <si>
-    <t>obtains; receives; gets</t>
-  </si>
-  <si>
-    <t>exhales; breathes out</t>
-  </si>
-  <si>
-    <t>breathes; inhales</t>
-  </si>
-  <si>
-    <t>wishes (for); desires; intends; plans</t>
-  </si>
-  <si>
-    <t>grabs hold (of); seizes; takes</t>
-  </si>
-  <si>
-    <t>advises; instructs; admonishes</t>
-  </si>
-  <si>
-    <t>understands; gets; lit. sees</t>
-  </si>
-  <si>
-    <t>leaves; abandons; gives up; forsakes</t>
-  </si>
-  <si>
-    <t>trains (in); trains (for the purpose of); practices (for the sake of); practice (to); lit. trains</t>
-  </si>
-  <si>
-    <t>uses; makes use (of); lit. associates</t>
-  </si>
-  <si>
-    <t>grows; increases</t>
-  </si>
-  <si>
-    <t>sets aside; lays aside; keeps; stores; saves; lit. throws down</t>
-  </si>
-  <si>
-    <t>associates (with); keeps company (with)</t>
-  </si>
-  <si>
-    <t>should; ought (to); is suitable (for); it is befitting (for)</t>
-  </si>
-  <si>
-    <t>gets; receives; obtains</t>
-  </si>
-  <si>
-    <t>remembers; recollects</t>
-  </si>
-  <si>
-    <t>sits; sits down</t>
-  </si>
-  <si>
-    <t>is; is being; becomes; exists</t>
-  </si>
-  <si>
-    <t>eats; chews; bites</t>
-  </si>
-  <si>
-    <t>leads (to); is useful (for); is conducive to</t>
-  </si>
-  <si>
-    <t>goes; walks; moves; wanders around</t>
-  </si>
-  <si>
-    <t>exerts oneself; strives; applies oneself; lit. puts forward</t>
-  </si>
-  <si>
-    <t>tries; makes an effort; strives for; exerts oneself</t>
-  </si>
-  <si>
-    <t>gets to; attains; finds; acquires; obtains; lit. goes up to</t>
-  </si>
-  <si>
-    <t>enjoys; finds high pleasure in</t>
-  </si>
-  <si>
-    <t>enters; goes into</t>
-  </si>
-  <si>
-    <t>lives (in); dwells (in)</t>
-  </si>
-  <si>
-    <t>grows; increases; multiplies</t>
-  </si>
-  <si>
     <t>sees</t>
   </si>
   <si>
@@ -2701,36 +2701,36 @@
     <t>farmer; ploughman</t>
   </si>
   <si>
+    <t>engages (in); practices; performs</t>
+  </si>
+  <si>
+    <t>arouses; exhibits; produces; brings into being</t>
+  </si>
+  <si>
+    <t>practices; follows a course of action; follows a method; is intent on</t>
+  </si>
+  <si>
+    <t>thinks; imagines; presumes</t>
+  </si>
+  <si>
+    <t>grasps; holds onto; clings to; takes as one's own; lit. takes near</t>
+  </si>
+  <si>
+    <t>is reborn in; re-arises; lit. goes towards</t>
+  </si>
+  <si>
+    <t>is disenchanted; is disinterested; is disillusioned</t>
+  </si>
+  <si>
+    <t>indulges (in); is addicted (to); lit. yokes oneself (to)</t>
+  </si>
+  <si>
+    <t>eats; consumes</t>
+  </si>
+  <si>
     <t>appears; arises; takes place</t>
   </si>
   <si>
-    <t>is reborn in; re-arises; lit. goes towards</t>
-  </si>
-  <si>
-    <t>engages (in); practices; performs</t>
-  </si>
-  <si>
-    <t>arouses; exhibits; produces; brings into being</t>
-  </si>
-  <si>
-    <t>practices; follows a course of action; follows a method; is intent on</t>
-  </si>
-  <si>
-    <t>thinks; imagines; presumes</t>
-  </si>
-  <si>
-    <t>grasps; holds onto; clings to; takes as one's own; lit. takes near</t>
-  </si>
-  <si>
-    <t>is disenchanted; is disinterested; is disillusioned</t>
-  </si>
-  <si>
-    <t>indulges (in); is addicted (to); lit. yokes oneself (to)</t>
-  </si>
-  <si>
-    <t>eats; consumes</t>
-  </si>
-  <si>
     <t>meditates; contemplates; lit. thinks</t>
   </si>
   <si>
@@ -2740,27 +2740,27 @@
     <t>causes; effects</t>
   </si>
   <si>
+    <t>there are; they are</t>
+  </si>
+  <si>
+    <t>we are</t>
+  </si>
+  <si>
+    <t>you are</t>
+  </si>
+  <si>
+    <t>you (all) must be; may you (all) be</t>
+  </si>
+  <si>
+    <t>I am</t>
+  </si>
+  <si>
     <t>they are; there are</t>
   </si>
   <si>
     <t>there is</t>
   </si>
   <si>
-    <t>there are; they are</t>
-  </si>
-  <si>
-    <t>we are</t>
-  </si>
-  <si>
-    <t>you are</t>
-  </si>
-  <si>
-    <t>you (all) must be; may you (all) be</t>
-  </si>
-  <si>
-    <t>I am</t>
-  </si>
-  <si>
     <t>addressed; said (to)</t>
   </si>
   <si>
@@ -2812,15 +2812,15 @@
     <t>monk; sage; hermit; holy man</t>
   </si>
   <si>
+    <t>rice</t>
+  </si>
+  <si>
+    <t>fire</t>
+  </si>
+  <si>
     <t>householder; landowner; lit. house master</t>
   </si>
   <si>
-    <t>rice</t>
-  </si>
-  <si>
-    <t>fire</t>
-  </si>
-  <si>
     <t>seer; sage</t>
   </si>
   <si>
@@ -2869,51 +2869,51 @@
     <t>one was; it was</t>
   </si>
   <si>
+    <t>excess; pleasure; intoxication</t>
+  </si>
+  <si>
+    <t>livelihood; way of earning a living</t>
+  </si>
+  <si>
+    <t>vigilance; earnestness; carefulness; conscientiousness; heedfulness</t>
+  </si>
+  <si>
+    <t>Awakened One; Buddha; who is wide awake; who has completely understood</t>
+  </si>
+  <si>
+    <t>false teaching; against the teaching</t>
+  </si>
+  <si>
     <t>skin</t>
   </si>
   <si>
-    <t>excess; pleasure; intoxication</t>
-  </si>
-  <si>
-    <t>vigilance; earnestness; carefulness; conscientiousness; heedfulness</t>
-  </si>
-  <si>
-    <t>livelihood; way of earning a living</t>
-  </si>
-  <si>
-    <t>Awakened One; Buddha; who is wide awake; who has completely understood</t>
-  </si>
-  <si>
-    <t>false teaching; against the teaching</t>
-  </si>
-  <si>
     <t>complete comprehension (of); total understanding (of); lit. arriving</t>
   </si>
   <si>
+    <t>my; mine</t>
+  </si>
+  <si>
+    <t>by me; with me</t>
+  </si>
+  <si>
+    <t>us (object)</t>
+  </si>
+  <si>
+    <t>for us; to us</t>
+  </si>
+  <si>
+    <t>we</t>
+  </si>
+  <si>
+    <t>our</t>
+  </si>
+  <si>
+    <t>our; of us</t>
+  </si>
+  <si>
     <t>by me</t>
   </si>
   <si>
-    <t>my; mine</t>
-  </si>
-  <si>
-    <t>by me; with me</t>
-  </si>
-  <si>
-    <t>us (object)</t>
-  </si>
-  <si>
-    <t>for us; to us</t>
-  </si>
-  <si>
-    <t>we</t>
-  </si>
-  <si>
-    <t>our</t>
-  </si>
-  <si>
-    <t>our; of us</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
@@ -2929,18 +2929,18 @@
     <t>leads; carries away; takes away</t>
   </si>
   <si>
+    <t>(negative particle); no; not</t>
+  </si>
+  <si>
+    <t>together (with); with</t>
+  </si>
+  <si>
+    <t>with; together (with); accompanied (by)</t>
+  </si>
+  <si>
     <t>then; now; indeed</t>
   </si>
   <si>
-    <t>(negative particle); no; not</t>
-  </si>
-  <si>
-    <t>together (with); with</t>
-  </si>
-  <si>
-    <t>with; together (with); accompanied (by)</t>
-  </si>
-  <si>
     <t>no; not</t>
   </si>
   <si>
@@ -2971,27 +2971,27 @@
     <t>will give (to)</t>
   </si>
   <si>
+    <t>to you all; for you all</t>
+  </si>
+  <si>
+    <t>by you all; with you all</t>
+  </si>
+  <si>
+    <t>of you all; yours</t>
+  </si>
+  <si>
+    <t>you (object)</t>
+  </si>
+  <si>
     <t>to you; for you all</t>
   </si>
   <si>
+    <t>you all; you (respectful plural) (object)</t>
+  </si>
+  <si>
     <t>you all; you (respectful plural)</t>
   </si>
   <si>
-    <t>you (object)</t>
-  </si>
-  <si>
-    <t>to you all; for you all</t>
-  </si>
-  <si>
-    <t>by you all; with you all</t>
-  </si>
-  <si>
-    <t>of you all; yours</t>
-  </si>
-  <si>
-    <t>you all; you (respectful plural) (object)</t>
-  </si>
-  <si>
     <t>you</t>
   </si>
   <si>
@@ -3043,12 +3043,12 @@
     <t>who returns once; once-returner</t>
   </si>
   <si>
+    <t>happy one; who is at ease; who is happy; who is comfortable</t>
+  </si>
+  <si>
     <t>celibate person; one living the holy life</t>
   </si>
   <si>
-    <t>happy one; who is at ease; who is happy; who is comfortable</t>
-  </si>
-  <si>
     <t>fellow monk; spiritual companion</t>
   </si>
   <si>
@@ -3061,30 +3061,30 @@
     <t>support (of); maintenance (of); looking after; lit. holding together</t>
   </si>
   <si>
+    <t>wise; insightful; percipient</t>
+  </si>
+  <si>
+    <t>powerful; strong</t>
+  </si>
+  <si>
+    <t>mindful; fully present; attentive; lit. having memory quality</t>
+  </si>
+  <si>
     <t>virtuous; observing the moral practices</t>
   </si>
   <si>
-    <t>wise; insightful; percipient</t>
-  </si>
-  <si>
-    <t>powerful; strong</t>
-  </si>
-  <si>
-    <t>mindful; fully present; attentive; lit. having memory quality</t>
-  </si>
-  <si>
     <t>unlearned; untaught; uninitiated; untrained; lit. one who has not heard</t>
   </si>
   <si>
+    <t>the Sublime One; the Blessed One; the Fortunate One; the Buddha</t>
+  </si>
+  <si>
+    <t>venerable; reverend; lit. elder; respected</t>
+  </si>
+  <si>
     <t>person with sight; who can see; lit. having eyes quality</t>
   </si>
   <si>
-    <t>the Sublime One; the Blessed One; the Fortunate One; the Buddha</t>
-  </si>
-  <si>
-    <t>venerable; reverend; lit. elder; respected</t>
-  </si>
-  <si>
     <t>teacher; master; the Buddha</t>
   </si>
   <si>
@@ -3109,12 +3109,12 @@
     <t>enjoys; indulges; has sex with; lit. walks around</t>
   </si>
   <si>
+    <t>at the right moment; at a suitable time; at the proper time</t>
+  </si>
+  <si>
     <t>or; either or</t>
   </si>
   <si>
-    <t>at the right moment; at a suitable time; at the proper time</t>
-  </si>
-  <si>
     <t>when; whenever; lit. at whichever time</t>
   </si>
   <si>
@@ -3178,24 +3178,24 @@
     <t>takes a bath; bathes; washes</t>
   </si>
   <si>
+    <t>could go; would move; could walk</t>
+  </si>
+  <si>
+    <t>could know; would understand; could be aware; would find out</t>
+  </si>
+  <si>
+    <t>could come; would come along; could approach; would arrive</t>
+  </si>
+  <si>
+    <t>should say; could speak</t>
+  </si>
+  <si>
+    <t>could get; would experience; would come across; lit. could arrive at</t>
+  </si>
+  <si>
     <t>could see; would see</t>
   </si>
   <si>
-    <t>could go; would move; could walk</t>
-  </si>
-  <si>
-    <t>could know; would understand; could be aware; would find out</t>
-  </si>
-  <si>
-    <t>could come; would come along; could approach; would arrive</t>
-  </si>
-  <si>
-    <t>should say; could speak</t>
-  </si>
-  <si>
-    <t>could get; would experience; would come across; lit. could arrive at</t>
-  </si>
-  <si>
     <t>could become available (for); would accrues (to); could crop up (for); lit. would arise (for)</t>
   </si>
   <si>
@@ -3214,60 +3214,60 @@
     <t>may be; would be; could be</t>
   </si>
   <si>
+    <t>training; practice</t>
+  </si>
+  <si>
+    <t>verse; poem; stanza; lit. in singing way</t>
+  </si>
+  <si>
+    <t>decay; aging</t>
+  </si>
+  <si>
+    <t>inquiry; judgement; investigation; discrimination</t>
+  </si>
+  <si>
+    <t>direction; point of the compass; cardinal point</t>
+  </si>
+  <si>
+    <t>wisdom; knowledge; insight</t>
+  </si>
+  <si>
+    <t>wishing; wanting; covetousness</t>
+  </si>
+  <si>
+    <t>army; multitude</t>
+  </si>
+  <si>
+    <t>branch</t>
+  </si>
+  <si>
+    <t>arm; forearm</t>
+  </si>
+  <si>
+    <t>(vinaya) appointing; indicating; designating; lit. pointing out</t>
+  </si>
+  <si>
+    <t>word; speech; statement; talk</t>
+  </si>
+  <si>
+    <t>craving; wanting; desire; lit. thirst</t>
+  </si>
+  <si>
+    <t>sensation; feeling; felt experience</t>
+  </si>
+  <si>
+    <t>tongue</t>
+  </si>
+  <si>
+    <t>female disciple; laywomen; female devotee</t>
+  </si>
+  <si>
+    <t>ordination; renunciation; becoming a monastic; lit. going forth</t>
+  </si>
+  <si>
     <t>personal experience; realization</t>
   </si>
   <si>
-    <t>ordination; renunciation; becoming a monastic; lit. going forth</t>
-  </si>
-  <si>
-    <t>training; practice</t>
-  </si>
-  <si>
-    <t>verse; poem; stanza; lit. in singing way</t>
-  </si>
-  <si>
-    <t>decay; aging</t>
-  </si>
-  <si>
-    <t>inquiry; judgement; investigation; discrimination</t>
-  </si>
-  <si>
-    <t>direction; point of the compass; cardinal point</t>
-  </si>
-  <si>
-    <t>wisdom; knowledge; insight</t>
-  </si>
-  <si>
-    <t>wishing; wanting; covetousness</t>
-  </si>
-  <si>
-    <t>army; multitude</t>
-  </si>
-  <si>
-    <t>branch</t>
-  </si>
-  <si>
-    <t>arm; forearm</t>
-  </si>
-  <si>
-    <t>(vinaya) appointing; indicating; designating; lit. pointing out</t>
-  </si>
-  <si>
-    <t>word; speech; statement; talk</t>
-  </si>
-  <si>
-    <t>craving; wanting; desire; lit. thirst</t>
-  </si>
-  <si>
-    <t>sensation; feeling; felt experience</t>
-  </si>
-  <si>
-    <t>tongue</t>
-  </si>
-  <si>
-    <t>female disciple; laywomen; female devotee</t>
-  </si>
-  <si>
     <t>people; population; generation; mankind</t>
   </si>
   <si>
@@ -3355,12 +3355,12 @@
     <t>daughter</t>
   </si>
   <si>
+    <t>coming; approaching</t>
+  </si>
+  <si>
     <t>undertaking; taking up; accepting</t>
   </si>
   <si>
-    <t>coming; approaching</t>
-  </si>
-  <si>
     <t>removing; getting rid of; giving up; driving out</t>
   </si>
   <si>
@@ -3382,33 +3382,33 @@
     <t>sitting down</t>
   </si>
   <si>
+    <t>stability; constancy; long lasting; persisting; lit. standing</t>
+  </si>
+  <si>
+    <t>hut</t>
+  </si>
+  <si>
+    <t>cleanness; purity (of); purification (of); holiness</t>
+  </si>
+  <si>
+    <t>(vinaya) offence; transgression</t>
+  </si>
+  <si>
     <t>view; belief; opinion; concept; theory; attitude</t>
   </si>
   <si>
+    <t>attainment; meditation achievement</t>
+  </si>
+  <si>
+    <t>liking; preference; inclination; approval; lit. pleasure</t>
+  </si>
+  <si>
+    <t>good destination; happy fate; heaven; lit. going well</t>
+  </si>
+  <si>
     <t>mindfulness; presence; recollection; awareness</t>
   </si>
   <si>
-    <t>stability; constancy; long lasting; persisting; lit. standing</t>
-  </si>
-  <si>
-    <t>hut</t>
-  </si>
-  <si>
-    <t>cleanness; purity (of); purification (of); holiness</t>
-  </si>
-  <si>
-    <t>(vinaya) offence; transgression</t>
-  </si>
-  <si>
-    <t>attainment; meditation achievement</t>
-  </si>
-  <si>
-    <t>liking; preference; inclination; approval; lit. pleasure</t>
-  </si>
-  <si>
-    <t>good destination; happy fate; heaven; lit. going well</t>
-  </si>
-  <si>
     <t>delight; heart-felt joy; rapture; joyful interest; bliss; lit. lovely feeling</t>
   </si>
   <si>
@@ -3439,12 +3439,12 @@
     <t>on one side</t>
   </si>
   <si>
+    <t>everywhere; in every place</t>
+  </si>
+  <si>
     <t>from where?; where?</t>
   </si>
   <si>
-    <t>everywhere; in every place</t>
-  </si>
-  <si>
     <t>there; in that place</t>
   </si>
   <si>
@@ -3493,129 +3493,129 @@
     <t>for alms; to collect alms food</t>
   </si>
   <si>
+    <t>being; living being</t>
+  </si>
+  <si>
+    <t>sense; mental faculty; power; lit. belonging to Inda</t>
+  </si>
+  <si>
+    <t>comfortable (for); lit. for the comfort (of); to the ease (of).</t>
+  </si>
+  <si>
+    <t>beneficial (for); advantageous (for); lit. for the benefit (of); to the blessing (of)</t>
+  </si>
+  <si>
+    <t>matter; material thing; materiality; experience of material world; physical objects of consciousness; first of the five aggregates</t>
+  </si>
+  <si>
+    <t>homelessness</t>
+  </si>
+  <si>
+    <t>household life; domestic life</t>
+  </si>
+  <si>
+    <t>ease; comfort; happiness; pleasure</t>
+  </si>
+  <si>
+    <t>welfare; good; benefit; blessing</t>
+  </si>
+  <si>
+    <t>mental objects of consciousness; mentality; mental factors of feeling, perception, intention, contact and attention; lit. name</t>
+  </si>
+  <si>
+    <t>vigour; energy; effort; valour; lit. state of a strong man</t>
+  </si>
+  <si>
+    <t>full development; maturity; completion; plenty; fullness</t>
+  </si>
+  <si>
+    <t>death</t>
+  </si>
+  <si>
+    <t>source; origin; foundation; reason; lit. tied down to</t>
+  </si>
+  <si>
+    <t>family; house; household; respectable family</t>
+  </si>
+  <si>
+    <t>joy; happiness; gladness</t>
+  </si>
+  <si>
+    <t>forest; wood</t>
+  </si>
+  <si>
+    <t>(Dhamma) power; strength</t>
+  </si>
+  <si>
+    <t>measure; measurement; length; size</t>
+  </si>
+  <si>
+    <t>acquisition; appropriation; taking possession; grasping; clinging; lit. taking near</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>side (of the body); flank</t>
+  </si>
+  <si>
+    <t>cloth; clothes; robe</t>
+  </si>
+  <si>
+    <t>merit; virtue; good deed; spiritual wealth</t>
+  </si>
+  <si>
+    <t>house; a dwelling place</t>
+  </si>
+  <si>
+    <t>in order to visit; for the purpose of seeing</t>
+  </si>
+  <si>
+    <t>present state of existence; earthly existence; such a state; lit. state of being here</t>
+  </si>
+  <si>
+    <t>source; origin; root</t>
+  </si>
+  <si>
+    <t>(mental) suffering; melancholy; dejection; depression; dissatisfaction</t>
+  </si>
+  <si>
+    <t>discomfort; suffering; pain; unease; unsatisfaction; problem; trouble</t>
+  </si>
+  <si>
+    <t>medicine; remedy; tonic; drug</t>
+  </si>
+  <si>
+    <t>not deteriorating; not decreasing; non-decline; non-regress</t>
+  </si>
+  <si>
+    <t>saying; speech; statement; utterance; talk; words; lit. what was said</t>
+  </si>
+  <si>
+    <t>(of mental defilement) complete quenching; total emancipation; complete cooling; lit. blowing away</t>
+  </si>
+  <si>
+    <t>shelter; refuge; help; lit. going to</t>
+  </si>
+  <si>
+    <t>fault; error; mistake; lit. to be avoided</t>
+  </si>
+  <si>
+    <t>precept; instruction; training rule; lit. part of training</t>
+  </si>
+  <si>
+    <t>danger; peril</t>
+  </si>
+  <si>
+    <t>eating; taking food</t>
+  </si>
+  <si>
     <t xml:space="preserve">which is not given; something not offered </t>
   </si>
   <si>
-    <t>precept; instruction; training rule; lit. part of training</t>
-  </si>
-  <si>
-    <t>danger; peril</t>
-  </si>
-  <si>
     <t>object of the eye; shape; sight</t>
   </si>
   <si>
-    <t>being; living being</t>
-  </si>
-  <si>
-    <t>sense; mental faculty; power; lit. belonging to Inda</t>
-  </si>
-  <si>
-    <t>comfortable (for); lit. for the comfort (of); to the ease (of).</t>
-  </si>
-  <si>
-    <t>beneficial (for); advantageous (for); lit. for the benefit (of); to the blessing (of)</t>
-  </si>
-  <si>
-    <t>matter; material thing; materiality; experience of material world; physical objects of consciousness; first of the five aggregates</t>
-  </si>
-  <si>
-    <t>homelessness</t>
-  </si>
-  <si>
-    <t>household life; domestic life</t>
-  </si>
-  <si>
-    <t>ease; comfort; happiness; pleasure</t>
-  </si>
-  <si>
-    <t>welfare; good; benefit; blessing</t>
-  </si>
-  <si>
-    <t>mental objects of consciousness; mentality; mental factors of feeling, perception, intention, contact and attention; lit. name</t>
-  </si>
-  <si>
-    <t>vigour; energy; effort; valour; lit. state of a strong man</t>
-  </si>
-  <si>
-    <t>full development; maturity; completion; plenty; fullness</t>
-  </si>
-  <si>
-    <t>death</t>
-  </si>
-  <si>
-    <t>source; origin; foundation; reason; lit. tied down to</t>
-  </si>
-  <si>
-    <t>family; house; household; respectable family</t>
-  </si>
-  <si>
-    <t>joy; happiness; gladness</t>
-  </si>
-  <si>
-    <t>(Dhamma) power; strength</t>
-  </si>
-  <si>
-    <t>forest; wood</t>
-  </si>
-  <si>
-    <t>measure; measurement; length; size</t>
-  </si>
-  <si>
-    <t>acquisition; appropriation; taking possession; grasping; clinging; lit. taking near</t>
-  </si>
-  <si>
-    <t>body</t>
-  </si>
-  <si>
-    <t>side (of the body); flank</t>
-  </si>
-  <si>
-    <t>cloth; clothes; robe</t>
-  </si>
-  <si>
-    <t>merit; virtue; good deed; spiritual wealth</t>
-  </si>
-  <si>
-    <t>house; a dwelling place</t>
-  </si>
-  <si>
-    <t>in order to visit; for the purpose of seeing</t>
-  </si>
-  <si>
-    <t>present state of existence; earthly existence; such a state; lit. state of being here</t>
-  </si>
-  <si>
-    <t>source; origin; root</t>
-  </si>
-  <si>
-    <t>(mental) suffering; melancholy; dejection; depression; dissatisfaction</t>
-  </si>
-  <si>
-    <t>discomfort; suffering; pain; unease; unsatisfaction; problem; trouble</t>
-  </si>
-  <si>
-    <t>medicine; remedy; tonic; drug</t>
-  </si>
-  <si>
-    <t>not deteriorating; not decreasing; non-decline; non-regress</t>
-  </si>
-  <si>
-    <t>saying; speech; statement; utterance; talk; words; lit. what was said</t>
-  </si>
-  <si>
-    <t>(of mental defilement) complete quenching; total emancipation; complete cooling; lit. blowing away</t>
-  </si>
-  <si>
-    <t>shelter; refuge; help; lit. going to</t>
-  </si>
-  <si>
-    <t>fault; error; mistake; lit. to be avoided</t>
-  </si>
-  <si>
-    <t>eating; taking food</t>
-  </si>
-  <si>
     <t>awareness; consciousness; fifth of the five aggregates; lit. knowing</t>
   </si>
   <si>
@@ -3706,34 +3706,34 @@
     <t>a bone</t>
   </si>
   <si>
+    <t>that much; that far; as long as; to that extent; until; at least</t>
+  </si>
+  <si>
+    <t>too; also; as well</t>
+  </si>
+  <si>
     <t>surely?; didn't?; wouldn't?</t>
   </si>
   <si>
     <t>it is suitable (to); it is proper (to); it is fit (for); lit. healthy</t>
   </si>
   <si>
+    <t>is able (to); is possible (to); is capable (of); lit. enough</t>
+  </si>
+  <si>
+    <t>how?; in what way?</t>
+  </si>
+  <si>
+    <t>enough; it is enough (for)</t>
+  </si>
+  <si>
+    <t>as long as; as far as; up to; until; from … to …</t>
+  </si>
+  <si>
+    <t>it is possible (to); one is able (to)</t>
+  </si>
+  <si>
     <t>(it is) suitable (to); proper (to); worthy (for); lit. enough (to)</t>
-  </si>
-  <si>
-    <t>that much; that far; as long as; to that extent; until; at least</t>
-  </si>
-  <si>
-    <t>too; also; as well</t>
-  </si>
-  <si>
-    <t>is able (to); is possible (to); is capable (of); lit. enough</t>
-  </si>
-  <si>
-    <t>how?; in what way?</t>
-  </si>
-  <si>
-    <t>enough; it is enough (for)</t>
-  </si>
-  <si>
-    <t>as long as; as far as; up to; until; from … to …</t>
-  </si>
-  <si>
-    <t>it is possible (to); one is able (to)</t>
   </si>
   <si>
     <t>that's enough (of)! stop (with)!</t>
@@ -7479,7 +7479,7 @@
         <v>191</v>
       </c>
       <c r="B188" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="C188" t="s">
         <v>824</v>
@@ -7564,7 +7564,7 @@
         <v>196</v>
       </c>
       <c r="B193" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C193" t="s">
         <v>829</v>
@@ -8975,7 +8975,7 @@
         <v>279</v>
       </c>
       <c r="B276" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="C276" t="s">
         <v>911</v>
@@ -9009,7 +9009,7 @@
         <v>281</v>
       </c>
       <c r="B278" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C278" t="s">
         <v>913</v>
@@ -9862,7 +9862,7 @@
         <v>623</v>
       </c>
       <c r="C328" t="s">
-        <v>963</v>
+        <v>958</v>
       </c>
       <c r="D328" t="s">
         <v>1271</v>
@@ -9879,7 +9879,7 @@
         <v>623</v>
       </c>
       <c r="C329" t="s">
-        <v>959</v>
+        <v>963</v>
       </c>
       <c r="D329" t="s">
         <v>1271</v>
@@ -11936,7 +11936,7 @@
         <v>633</v>
       </c>
       <c r="C450" t="s">
-        <v>1083</v>
+        <v>663</v>
       </c>
       <c r="D450" t="s">
         <v>1289</v>
@@ -11953,7 +11953,7 @@
         <v>633</v>
       </c>
       <c r="C451" t="s">
-        <v>677</v>
+        <v>1083</v>
       </c>
       <c r="D451" t="s">
         <v>1289</v>

</xml_diff>